<commit_message>
update eqcost import template
</commit_message>
<xml_diff>
--- a/doc/开发实际模板/设备成本表.xlsx
+++ b/doc/开发实际模板/设备成本表.xlsx
@@ -50,7 +50,7 @@
     <definedName name="park">[6]停车场!#REF!</definedName>
     <definedName name="PC">[7]p2!$D$36</definedName>
     <definedName name="PDS">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'P3-BJ'!$B$1:$M$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'P3-BJ'!$B$1:$O$34</definedName>
     <definedName name="Print_Area_MI">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'P3-BJ'!$1:$8</definedName>
     <definedName name="Printer">[7]p2!$D$37</definedName>
@@ -91,14 +91,14 @@
     <definedName name="填表日期">[9]P1!$G$5</definedName>
     <definedName name="项目名称">[9]P1!$G$7</definedName>
     <definedName name="销售员">[9]P1!$W$5</definedName>
-    <definedName name="自主设备合计">'P3-BJ'!$L$6</definedName>
+    <definedName name="自主设备合计">'P3-BJ'!$N$6</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t xml:space="preserve">同方泰德智能科技（上海）有限公司 </t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -225,6 +225,82 @@
   </si>
   <si>
     <t>TAI</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>物料类别</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>税收类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WW3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WW4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WW5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WW6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NNN3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NNN4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NNN5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NNN6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GGG3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GGG4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GGG5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GGG6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>电子类</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>通信类</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>家居类</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>增值税</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>非增值税</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1323,12 +1399,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
@@ -1349,6 +1419,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="116">
@@ -25338,12 +25414,12 @@
   <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:R69"/>
+  <dimension ref="B1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AE3" sqref="AE3"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomLeft" activeCell="O12" sqref="O12:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -25358,56 +25434,62 @@
     <col min="8" max="8" width="13.25" style="6" customWidth="1"/>
     <col min="9" max="9" width="10.875" style="7" customWidth="1"/>
     <col min="10" max="10" width="7.125" style="55" customWidth="1"/>
-    <col min="11" max="11" width="11.25" style="7" customWidth="1"/>
-    <col min="12" max="12" width="14.125" style="7" customWidth="1"/>
-    <col min="13" max="13" width="14.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="2.375" customWidth="1"/>
+    <col min="11" max="13" width="11.25" style="7" customWidth="1"/>
+    <col min="14" max="14" width="14.125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="14.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="2.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="C1" s="58" t="s">
+    <row r="1" spans="2:17" ht="20.100000000000001" customHeight="1">
+      <c r="C1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="2"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="C2" s="59" t="s">
+    <row r="2" spans="2:17" ht="20.100000000000001" customHeight="1">
+      <c r="C2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="3"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="2:15" ht="14.1" customHeight="1">
+    <row r="3" spans="2:17" ht="14.1" customHeight="1">
       <c r="E3" s="5"/>
       <c r="J3" s="8"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="2:15" ht="14.1" customHeight="1">
+    <row r="4" spans="2:17" ht="14.1" customHeight="1">
       <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
@@ -25419,14 +25501,16 @@
       <c r="K4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="11" t="str">
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="11" t="str">
         <f>销售员</f>
         <v>刘谢方</v>
       </c>
-      <c r="M4" s="13"/>
-      <c r="N4" s="60"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="58"/>
     </row>
-    <row r="5" spans="2:15" ht="14.1" customHeight="1">
+    <row r="5" spans="2:17" ht="14.1" customHeight="1">
       <c r="B5" s="14"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
@@ -25444,14 +25528,16 @@
       <c r="K5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="16">
         <f>填表日期</f>
         <v>41050</v>
       </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="61"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="59"/>
     </row>
-    <row r="6" spans="2:15" ht="14.1" customHeight="1">
+    <row r="6" spans="2:17" ht="14.1" customHeight="1">
       <c r="B6" s="24" t="s">
         <v>19</v>
       </c>
@@ -25464,14 +25550,16 @@
       <c r="I6" s="27"/>
       <c r="J6" s="28"/>
       <c r="K6" s="27"/>
-      <c r="L6" s="29">
-        <f>SUM(L9:L18)</f>
-        <v>30900</v>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="29">
+        <f>SUM(N9:N18)</f>
+        <v>92700</v>
       </c>
-      <c r="M6" s="30"/>
-      <c r="N6" s="62"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="60"/>
     </row>
-    <row r="7" spans="2:15" ht="14.1" customHeight="1">
+    <row r="7" spans="2:17" ht="14.1" customHeight="1">
       <c r="B7" s="14"/>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -25483,10 +25571,12 @@
       <c r="J7" s="20"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
     </row>
-    <row r="8" spans="2:15" ht="14.1" customHeight="1">
+    <row r="8" spans="2:17" ht="14.1" customHeight="1">
       <c r="B8" s="21" t="s">
         <v>6</v>
       </c>
@@ -25518,14 +25608,20 @@
         <v>18</v>
       </c>
       <c r="L8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="O8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="63"/>
+      <c r="P8" s="61"/>
     </row>
-    <row r="9" spans="2:15" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="9" spans="2:17" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B9" s="31">
         <v>1</v>
       </c>
@@ -25557,16 +25653,22 @@
         <f>ROUNDUP(I9*J9,2)</f>
         <v>1545</v>
       </c>
-      <c r="L9" s="38">
+      <c r="L9" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="38">
         <f>K9*G9</f>
         <v>15450</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="O9" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="64"/>
+      <c r="P9" s="62"/>
     </row>
-    <row r="10" spans="2:15" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="10" spans="2:17" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B10" s="31">
         <v>2</v>
       </c>
@@ -25598,120 +25700,210 @@
         <f>ROUNDUP(I10*J10,2)</f>
         <v>1545</v>
       </c>
-      <c r="L10" s="38">
+      <c r="L10" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="N10" s="38">
         <f>K10*G10</f>
         <v>15450</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="O10" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="N10" s="64"/>
+      <c r="P10" s="62"/>
     </row>
-    <row r="11" spans="2:15" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="11" spans="2:17" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B11" s="31">
         <v>3</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="35">
+        <v>10</v>
+      </c>
+      <c r="H11" s="35">
+        <v>2000</v>
+      </c>
+      <c r="I11" s="36">
+        <v>1500</v>
+      </c>
       <c r="J11" s="37">
         <v>1.03</v>
       </c>
       <c r="K11" s="38">
         <f>ROUNDUP(I11*J11,2)</f>
-        <v>0</v>
+        <v>1545</v>
       </c>
-      <c r="L11" s="38">
+      <c r="L11" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="38">
         <f>K11*G11</f>
-        <v>0</v>
+        <v>15450</v>
       </c>
-      <c r="M11" s="32" t="s">
+      <c r="O11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="64"/>
+      <c r="P11" s="62"/>
     </row>
-    <row r="12" spans="2:15" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="12" spans="2:17" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B12" s="31">
         <v>4</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="36"/>
+      <c r="C12" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="35">
+        <v>10</v>
+      </c>
+      <c r="H12" s="35">
+        <v>2000</v>
+      </c>
+      <c r="I12" s="36">
+        <v>1500</v>
+      </c>
       <c r="J12" s="37">
         <v>1.03</v>
       </c>
       <c r="K12" s="38">
         <f>ROUNDUP(I12*J12,2)</f>
-        <v>0</v>
+        <v>1545</v>
       </c>
-      <c r="L12" s="38">
+      <c r="L12" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" s="38">
         <f>K12*G12</f>
-        <v>0</v>
+        <v>15450</v>
       </c>
-      <c r="M12" s="32" t="s">
+      <c r="O12" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="64"/>
+      <c r="P12" s="62"/>
     </row>
-    <row r="13" spans="2:15" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="13" spans="2:17" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B13" s="31">
         <v>5</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="36"/>
+      <c r="C13" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="35">
+        <v>10</v>
+      </c>
+      <c r="H13" s="35">
+        <v>2000</v>
+      </c>
+      <c r="I13" s="36">
+        <v>1500</v>
+      </c>
       <c r="J13" s="37">
         <v>1.03</v>
       </c>
       <c r="K13" s="38">
         <f t="shared" ref="K13:K18" si="0">ROUNDUP(I13*J13,2)</f>
-        <v>0</v>
+        <v>1545</v>
       </c>
-      <c r="L13" s="38">
-        <f t="shared" ref="L13:L18" si="1">K13*G13</f>
-        <v>0</v>
+      <c r="L13" s="38" t="s">
+        <v>48</v>
       </c>
-      <c r="M13" s="32"/>
-      <c r="N13" s="64"/>
+      <c r="M13" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="38">
+        <f t="shared" ref="N13:N18" si="1">K13*G13</f>
+        <v>15450</v>
+      </c>
+      <c r="O13" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" s="62"/>
     </row>
-    <row r="14" spans="2:15" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="14" spans="2:17" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B14" s="31">
         <v>6</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="38"/>
+      <c r="C14" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="35">
+        <v>10</v>
+      </c>
+      <c r="H14" s="35">
+        <v>2000</v>
+      </c>
+      <c r="I14" s="36">
+        <v>1500</v>
+      </c>
       <c r="J14" s="37">
         <v>1.03</v>
       </c>
       <c r="K14" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1545</v>
       </c>
-      <c r="L14" s="38">
+      <c r="L14" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="N14" s="38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15450</v>
       </c>
-      <c r="M14" s="32"/>
-      <c r="N14" s="64"/>
+      <c r="O14" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="P14" s="62"/>
     </row>
-    <row r="15" spans="2:15" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="15" spans="2:17" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B15" s="31">
         <v>7</v>
       </c>
@@ -25729,14 +25921,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="38">
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M15" s="32"/>
-      <c r="N15" s="64"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="62"/>
     </row>
-    <row r="16" spans="2:15" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="16" spans="2:17" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B16" s="31">
         <v>8</v>
       </c>
@@ -25754,14 +25948,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L16" s="38">
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M16" s="32"/>
-      <c r="N16" s="64"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="62"/>
     </row>
-    <row r="17" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="17" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B17" s="31">
         <v>9</v>
       </c>
@@ -25779,14 +25975,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L17" s="38">
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M17" s="32"/>
-      <c r="N17" s="64"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="62"/>
     </row>
-    <row r="18" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="18" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B18" s="31">
         <v>10</v>
       </c>
@@ -25804,14 +26002,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L18" s="38">
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M18" s="32"/>
-      <c r="N18" s="64"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="62"/>
     </row>
-    <row r="19" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="19" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B19" s="45">
         <v>1</v>
       </c>
@@ -25829,14 +26029,16 @@
         <f t="shared" ref="K19:K30" si="2">J19*I19</f>
         <v>0</v>
       </c>
-      <c r="L19" s="51">
-        <f t="shared" ref="L19:L30" si="3">G19*K19</f>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51">
+        <f t="shared" ref="N19:N30" si="3">G19*K19</f>
         <v>0</v>
       </c>
-      <c r="M19" s="52"/>
-      <c r="N19" s="65"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="63"/>
     </row>
-    <row r="20" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="20" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B20" s="45">
         <v>2</v>
       </c>
@@ -25854,14 +26056,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L20" s="51">
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M20" s="52"/>
-      <c r="N20" s="65"/>
+      <c r="O20" s="52"/>
+      <c r="P20" s="63"/>
     </row>
-    <row r="21" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="21" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B21" s="45">
         <v>3</v>
       </c>
@@ -25879,14 +26083,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L21" s="51">
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M21" s="52"/>
-      <c r="N21" s="65"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="63"/>
     </row>
-    <row r="22" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="22" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B22" s="45">
         <v>4</v>
       </c>
@@ -25904,14 +26110,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L22" s="51">
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M22" s="52"/>
-      <c r="N22" s="65"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="63"/>
     </row>
-    <row r="23" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="23" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B23" s="45">
         <v>5</v>
       </c>
@@ -25929,14 +26137,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L23" s="51">
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M23" s="52"/>
-      <c r="N23" s="65"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="63"/>
     </row>
-    <row r="24" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="24" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B24" s="45">
         <v>6</v>
       </c>
@@ -25954,14 +26164,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L24" s="51">
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M24" s="52"/>
-      <c r="N24" s="65"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="63"/>
     </row>
-    <row r="25" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="25" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B25" s="45">
         <v>7</v>
       </c>
@@ -25979,14 +26191,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L25" s="51">
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M25" s="52"/>
-      <c r="N25" s="65"/>
+      <c r="O25" s="52"/>
+      <c r="P25" s="63"/>
     </row>
-    <row r="26" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="26" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B26" s="45">
         <v>8</v>
       </c>
@@ -26004,14 +26218,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L26" s="51">
+      <c r="L26" s="51"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M26" s="52"/>
-      <c r="N26" s="65"/>
+      <c r="O26" s="52"/>
+      <c r="P26" s="63"/>
     </row>
-    <row r="27" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="27" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B27" s="45">
         <v>9</v>
       </c>
@@ -26029,14 +26245,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L27" s="51">
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M27" s="52"/>
-      <c r="N27" s="65"/>
+      <c r="O27" s="52"/>
+      <c r="P27" s="63"/>
     </row>
-    <row r="28" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="28" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B28" s="45">
         <v>10</v>
       </c>
@@ -26054,14 +26272,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L28" s="51">
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M28" s="52"/>
-      <c r="N28" s="65"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="63"/>
     </row>
-    <row r="29" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="29" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B29" s="45">
         <v>11</v>
       </c>
@@ -26079,14 +26299,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L29" s="51">
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M29" s="52"/>
-      <c r="N29" s="65"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="63"/>
     </row>
-    <row r="30" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="30" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B30" s="45">
         <v>12</v>
       </c>
@@ -26104,14 +26326,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L30" s="51">
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M30" s="52"/>
-      <c r="N30" s="65"/>
+      <c r="O30" s="52"/>
+      <c r="P30" s="63"/>
     </row>
-    <row r="31" spans="2:14" ht="14.1" customHeight="1" outlineLevel="1">
+    <row r="31" spans="2:16" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="B31" s="40"/>
       <c r="C31" s="41" t="s">
         <v>15</v>
@@ -26126,14 +26350,16 @@
       <c r="K31" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="L31" s="38">
-        <f>SUM(L9:L30)</f>
-        <v>30900</v>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38">
+        <f>SUM(N9:N30)</f>
+        <v>92700</v>
       </c>
-      <c r="M31" s="39"/>
-      <c r="N31" s="66"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="64"/>
     </row>
-    <row r="32" spans="2:14" ht="14.1" customHeight="1">
+    <row r="32" spans="2:16" ht="14.1" customHeight="1">
       <c r="B32" s="14"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
@@ -26145,10 +26371,12 @@
       <c r="J32" s="20"/>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
     </row>
-    <row r="33" spans="2:18" ht="14.1" customHeight="1">
+    <row r="33" spans="2:20" ht="14.1" customHeight="1">
       <c r="B33" s="14"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
@@ -26160,10 +26388,12 @@
       <c r="J33" s="20"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
     </row>
-    <row r="34" spans="2:18" ht="14.1" customHeight="1">
+    <row r="34" spans="2:20" ht="14.1" customHeight="1">
       <c r="B34" s="14"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -26175,22 +26405,26 @@
       <c r="J34" s="20"/>
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
     </row>
-    <row r="35" spans="2:18" ht="14.1" customHeight="1">
+    <row r="35" spans="2:20" ht="14.1" customHeight="1">
       <c r="E35" s="6"/>
       <c r="G35" s="53"/>
       <c r="H35" s="53"/>
       <c r="I35" s="54"/>
       <c r="J35" s="53"/>
       <c r="K35" s="53"/>
-      <c r="L35" s="12"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35" s="1"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="53"/>
+      <c r="N35" s="12"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="36" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="6"/>
@@ -26200,14 +26434,16 @@
       <c r="I36" s="54"/>
       <c r="J36" s="53"/>
       <c r="K36" s="53"/>
-      <c r="L36" s="12"/>
-      <c r="M36"/>
-      <c r="N36"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="53"/>
+      <c r="N36" s="12"/>
+      <c r="O36"/>
       <c r="P36"/>
-      <c r="Q36"/>
       <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
     </row>
-    <row r="37" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="37" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="6"/>
@@ -26217,14 +26453,16 @@
       <c r="I37" s="54"/>
       <c r="J37" s="53"/>
       <c r="K37" s="53"/>
-      <c r="L37" s="12"/>
-      <c r="M37"/>
-      <c r="N37"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="12"/>
+      <c r="O37"/>
       <c r="P37"/>
-      <c r="Q37"/>
       <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
     </row>
-    <row r="38" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="38" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="6"/>
@@ -26234,14 +26472,16 @@
       <c r="I38" s="54"/>
       <c r="J38" s="53"/>
       <c r="K38" s="53"/>
-      <c r="L38" s="12"/>
-      <c r="M38"/>
-      <c r="N38"/>
+      <c r="L38" s="53"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="12"/>
+      <c r="O38"/>
       <c r="P38"/>
-      <c r="Q38"/>
       <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
     </row>
-    <row r="39" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="39" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="12"/>
@@ -26252,12 +26492,14 @@
       <c r="J39" s="55"/>
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
-      <c r="O39"/>
-      <c r="P39"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
       <c r="Q39"/>
       <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
     </row>
-    <row r="40" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="40" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="12"/>
@@ -26268,12 +26510,14 @@
       <c r="J40" s="55"/>
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
-      <c r="O40"/>
-      <c r="P40"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
       <c r="Q40"/>
       <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
     </row>
-    <row r="41" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="41" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="12"/>
@@ -26284,12 +26528,14 @@
       <c r="J41" s="55"/>
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
-      <c r="O41"/>
-      <c r="P41"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
       <c r="Q41"/>
       <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
     </row>
-    <row r="42" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="42" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="12"/>
@@ -26300,12 +26546,14 @@
       <c r="J42" s="55"/>
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
-      <c r="O42"/>
-      <c r="P42"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
       <c r="Q42"/>
       <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
     </row>
-    <row r="43" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="43" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="12"/>
@@ -26316,12 +26564,14 @@
       <c r="J43" s="55"/>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
-      <c r="O43"/>
-      <c r="P43"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
       <c r="Q43"/>
       <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
     </row>
-    <row r="44" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="44" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="12"/>
@@ -26332,12 +26582,14 @@
       <c r="J44" s="55"/>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
-      <c r="O44"/>
-      <c r="P44"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
       <c r="Q44"/>
       <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
     </row>
-    <row r="45" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="45" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="12"/>
@@ -26348,12 +26600,14 @@
       <c r="J45" s="55"/>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
-      <c r="O45"/>
-      <c r="P45"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
       <c r="Q45"/>
       <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
     </row>
-    <row r="46" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="46" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="12"/>
@@ -26364,12 +26618,14 @@
       <c r="J46" s="55"/>
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
-      <c r="O46"/>
-      <c r="P46"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
       <c r="Q46"/>
       <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
     </row>
-    <row r="47" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="47" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="12"/>
@@ -26380,12 +26636,14 @@
       <c r="J47" s="55"/>
       <c r="K47" s="7"/>
       <c r="L47" s="7"/>
-      <c r="O47"/>
-      <c r="P47"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
       <c r="Q47"/>
       <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
     </row>
-    <row r="48" spans="2:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="48" spans="2:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="12"/>
@@ -26396,12 +26654,14 @@
       <c r="J48" s="55"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
-      <c r="O48"/>
-      <c r="P48"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
       <c r="Q48"/>
       <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
     </row>
-    <row r="49" spans="3:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="49" spans="3:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="12"/>
@@ -26412,12 +26672,14 @@
       <c r="J49" s="55"/>
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
-      <c r="O49"/>
-      <c r="P49"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
       <c r="Q49"/>
       <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
     </row>
-    <row r="50" spans="3:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="50" spans="3:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="12"/>
@@ -26428,12 +26690,14 @@
       <c r="J50" s="55"/>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
-      <c r="O50"/>
-      <c r="P50"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
       <c r="Q50"/>
       <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
     </row>
-    <row r="51" spans="3:18" s="1" customFormat="1" ht="14.1" customHeight="1">
+    <row r="51" spans="3:20" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="12"/>
@@ -26444,24 +26708,26 @@
       <c r="J51" s="55"/>
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
-      <c r="O51"/>
-      <c r="P51"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
       <c r="Q51"/>
       <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
     </row>
-    <row r="52" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="53" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="54" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="55" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="56" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="57" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="58" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="59" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="60" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="61" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="62" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="63" spans="3:18" ht="14.1" customHeight="1"/>
-    <row r="64" spans="3:18" ht="14.1" customHeight="1"/>
+    <row r="52" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="53" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="54" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="55" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="56" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="57" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="58" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="59" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="60" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="61" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="62" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="63" spans="3:20" ht="14.1" customHeight="1"/>
+    <row r="64" spans="3:20" ht="14.1" customHeight="1"/>
     <row r="65" ht="14.1" customHeight="1"/>
     <row r="66" ht="14.1" customHeight="1"/>
     <row r="67" ht="14.1" customHeight="1"/>
@@ -26474,8 +26740,8 @@
     <protectedRange sqref="E24:E25" name="区域1_1_3"/>
   </protectedRanges>
   <mergeCells count="2">
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="C2:O2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J9:J30">
@@ -26483,13 +26749,13 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:I30 K19:L30">
+  <conditionalFormatting sqref="C19:I30 K19:N30">
     <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"查询不到！"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M19:N31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O19:P31">
       <formula1>"同方上海库存,同方北京库存,同方代为采购"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>